<commit_message>
Class diagrams minor change and self-assessment done
</commit_message>
<xml_diff>
--- a/selfAssessment_Sprint3.xlsx
+++ b/selfAssessment_Sprint3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaosilva/Documents/GitHub/lei-24-s2-1dm-g132/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jles0\Documentos\ISEP\LEI\2º_semestre\Projeto\Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA41212-DF95-8C45-A6E5-2F6125FA4013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F71250-7193-4AD2-AAAD-503143033B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="880" windowWidth="26700" windowHeight="17760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="63">
   <si>
     <t>TeamID #</t>
   </si>
@@ -1482,37 +1482,37 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="12" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="6.296875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="12" width="7.796875" customWidth="1"/>
     <col min="13" max="13" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1523,13 +1523,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:13" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:13" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="58" t="s">
@@ -1544,7 +1544,7 @@
       <c r="L8" s="59"/>
       <c r="M8" s="60"/>
     </row>
-    <row r="9" spans="1:13" ht="106" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="106.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="29" t="str">
@@ -1583,27 +1583,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+      <c r="D10" s="53">
+        <v>4</v>
+      </c>
+      <c r="E10" s="26">
+        <v>4</v>
+      </c>
+      <c r="F10" s="27">
+        <v>4</v>
+      </c>
+      <c r="G10" s="27">
+        <v>3</v>
+      </c>
+      <c r="H10" s="27">
+        <v>2</v>
+      </c>
+      <c r="I10" s="27">
+        <v>2</v>
+      </c>
+      <c r="J10" s="27">
+        <v>4</v>
+      </c>
       <c r="K10" s="25"/>
-      <c r="L10" s="35" t="e">
+      <c r="L10" s="35">
         <f t="shared" ref="L10:L17" si="0">AVERAGE(D10:K10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3.2857142857142856</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="56"/>
       <c r="C11" s="25" t="s">
         <v>41</v>
@@ -1621,7 +1635,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="56"/>
       <c r="C12" s="6" t="s">
         <v>42</v>
@@ -1649,7 +1663,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="56"/>
       <c r="C13" s="6" t="s">
         <v>43</v>
@@ -1667,7 +1681,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="56"/>
       <c r="C14" s="6" t="s">
         <v>44</v>
@@ -1685,7 +1699,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="56"/>
       <c r="C15" s="6" t="s">
         <v>45</v>
@@ -1703,7 +1717,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="56"/>
       <c r="C16" s="6" t="s">
         <v>62</v>
@@ -1733,7 +1747,7 @@
         <v>4.666666666666667</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="57"/>
       <c r="C17" s="28" t="s">
         <v>6</v>
@@ -1751,38 +1765,38 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="33">
         <f t="shared" ref="D18:K18" si="1">AVERAGE(D10:D17)</f>
-        <v>5</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="E18" s="33">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="F18" s="33">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="G18" s="33">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="H18" s="33">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I18" s="33">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J18" s="33">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="K18" s="34" t="e">
         <f t="shared" si="1"/>
@@ -1790,7 +1804,7 @@
       </c>
       <c r="L18" s="38"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="42" t="s">
         <v>7</v>
       </c>
@@ -1806,7 +1820,7 @@
       <c r="K20" s="43"/>
       <c r="L20" s="44"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="45" t="s">
         <v>33</v>
       </c>
@@ -1822,7 +1836,7 @@
       <c r="K21" s="46"/>
       <c r="L21" s="47"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="48" t="s">
         <v>34</v>
       </c>
@@ -1838,7 +1852,7 @@
       <c r="K22" s="46"/>
       <c r="L22" s="47"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="45" t="s">
         <v>35</v>
       </c>
@@ -1854,7 +1868,7 @@
       <c r="K23" s="46"/>
       <c r="L23" s="47"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="45"/>
       <c r="B24" s="46"/>
       <c r="C24" s="46"/>
@@ -1868,7 +1882,7 @@
       <c r="K24" s="46"/>
       <c r="L24" s="47"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="49" t="s">
         <v>36</v>
       </c>
@@ -1884,7 +1898,7 @@
       <c r="K25" s="46"/>
       <c r="L25" s="47"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="45">
         <v>0</v>
       </c>
@@ -1902,7 +1916,7 @@
       <c r="K26" s="46"/>
       <c r="L26" s="47"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="45">
         <v>1</v>
       </c>
@@ -1920,7 +1934,7 @@
       <c r="K27" s="46"/>
       <c r="L27" s="47"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="45">
         <v>2</v>
       </c>
@@ -1938,7 +1952,7 @@
       <c r="K28" s="46"/>
       <c r="L28" s="47"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="45">
         <v>3</v>
       </c>
@@ -1956,7 +1970,7 @@
       <c r="K29" s="46"/>
       <c r="L29" s="47"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="45">
         <v>4</v>
       </c>
@@ -1974,7 +1988,7 @@
       <c r="K30" s="46"/>
       <c r="L30" s="47"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="45">
         <v>5</v>
       </c>
@@ -1992,7 +2006,7 @@
       <c r="K31" s="46"/>
       <c r="L31" s="47"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="50"/>
       <c r="B32" s="51"/>
       <c r="C32" s="51"/>
@@ -2026,25 +2040,25 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="55" t="s">
         <v>15</v>
       </c>
@@ -2076,7 +2090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="56"/>
       <c r="B4" s="64"/>
       <c r="C4" s="64"/>
@@ -2100,7 +2114,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="56"/>
       <c r="B5" s="64"/>
       <c r="C5" s="64"/>
@@ -2124,7 +2138,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>46</v>
       </c>
@@ -2150,7 +2164,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>47</v>
       </c>
@@ -2180,7 +2194,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>48</v>
       </c>
@@ -2206,7 +2220,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>49</v>
       </c>
@@ -2232,7 +2246,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>50</v>
       </c>
@@ -2258,7 +2272,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>51</v>
       </c>
@@ -2284,12 +2298,16 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
+      <c r="B12" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="18">
+        <v>4</v>
+      </c>
       <c r="D12" s="40"/>
       <c r="E12" s="11" t="s">
         <v>25</v>
@@ -2310,12 +2328,16 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
+      <c r="B13" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="18">
+        <v>4</v>
+      </c>
       <c r="D13" s="40"/>
       <c r="E13" s="11" t="s">
         <v>25</v>
@@ -2336,12 +2358,16 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
+      <c r="B14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="18">
+        <v>4</v>
+      </c>
       <c r="D14" s="40"/>
       <c r="E14" s="11" t="s">
         <v>25</v>
@@ -2362,7 +2388,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>55</v>
       </c>
@@ -2392,7 +2418,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>56</v>
       </c>
@@ -2422,7 +2448,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>57</v>
       </c>
@@ -2452,7 +2478,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>58</v>
       </c>
@@ -2478,7 +2504,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>59</v>
       </c>
@@ -2510,7 +2536,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>60</v>
       </c>
@@ -2540,7 +2566,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -2564,7 +2590,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -2588,7 +2614,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -2612,7 +2638,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -2636,7 +2662,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -2660,7 +2686,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -2684,7 +2710,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -2708,7 +2734,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
@@ -2732,7 +2758,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
@@ -2756,7 +2782,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>38</v>
       </c>
@@ -2782,7 +2808,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -2806,7 +2832,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="15"/>
       <c r="B32" s="39"/>
       <c r="C32" s="18"/>
@@ -2865,6 +2891,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -3048,22 +3089,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3079,28 +3129,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>